<commit_message>
Implemented projection approximations both for XB and Chain. Trouble with Chain version still (buckets full).
Co-authored-by: Anna Blume Jakobsen <201907691@post.au.dk>
</commit_message>
<xml_diff>
--- a/lockstep_algorithm/Results.xlsx
+++ b/lockstep_algorithm/Results.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ablum\Symbolic-SCCs\lockstep_algorithm\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rsmj9\Documents\Datalogi\8. Semester\SCC Project\Code\Symbolic-SCCs\lockstep_algorithm\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B1EDF4-A881-4DE7-B41F-204A53331FDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F816F741-6EFE-4294-ABCD-CE1B5100D90F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{39485520-4A0B-427E-9E64-4FED19D4A5EB}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{39485520-4A0B-427E-9E64-4FED19D4A5EB}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -85,7 +85,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
@@ -190,7 +190,7 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -524,7 +524,7 @@
   <dimension ref="A1:X24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1587,6 +1587,10 @@
     </row>
     <row r="16" spans="1:24" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="9"/>
+      <c r="D16" s="10">
+        <f>SUM(D2:D15)</f>
+        <v>352</v>
+      </c>
       <c r="E16" s="9">
         <f>SUM(E2:E15)</f>
         <v>106310</v>

</xml_diff>